<commit_message>
actualizacion excel e insert en limites y bloqueos
actualizacion excel  e insert datos en limites bloqueos
</commit_message>
<xml_diff>
--- a/diagrams/bdrelacionadas.xlsx
+++ b/diagrams/bdrelacionadas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITM\BDAVANZADAS\Repositorio\bet_itm_assignment\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4913ECC7-B4E8-4C99-AE2D-58FF7AB3FB05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2AE6FD-2945-4BDD-8C8D-238F5625F84D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{16A54CA9-296D-4623-BA6E-D4D5AADD1692}"/>
+    <workbookView xWindow="18840" yWindow="2676" windowWidth="7500" windowHeight="6000" activeTab="1" xr2:uid="{16A54CA9-296D-4623-BA6E-D4D5AADD1692}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfico1" sheetId="3" r:id="rId1"/>
@@ -6701,8 +6701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780A45B2-831B-4F5B-8807-F78F0F606349}">
   <dimension ref="B2:P39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7067,7 +7067,7 @@
       <c r="J19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="L19" s="13" t="s">
         <v>34</v>
       </c>
       <c r="N19" s="5"/>

</xml_diff>

<commit_message>
ACTUALIZACION EXCEL  Y TABLA SESIONES
A
</commit_message>
<xml_diff>
--- a/diagrams/bdrelacionadas.xlsx
+++ b/diagrams/bdrelacionadas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITM\BDAVANZADAS\Repositorio\bet_itm_assignment\diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B30F134-9DFC-43E2-9747-8081345B8D30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B19A22-39C8-4033-9D75-0CDF454C51A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{16A54CA9-296D-4623-BA6E-D4D5AADD1692}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" activeTab="1" xr2:uid="{16A54CA9-296D-4623-BA6E-D4D5AADD1692}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfico1" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="144">
   <si>
     <t>usuarios</t>
   </si>
@@ -466,6 +466,18 @@
   </si>
   <si>
     <t>fecha_ultima_modificacion</t>
+  </si>
+  <si>
+    <t>sesiones</t>
+  </si>
+  <si>
+    <t>idusuario</t>
+  </si>
+  <si>
+    <t>fecha_inicio_sesion</t>
+  </si>
+  <si>
+    <t>IP</t>
   </si>
 </sst>
 </file>
@@ -596,10 +608,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6699,7 +6711,7 @@
   <dimension ref="B2:P39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="N22" sqref="N22:N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6711,7 +6723,7 @@
     <col min="10" max="10" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
     <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.6640625" customWidth="1"/>
     <col min="16" max="16" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6720,13 +6732,13 @@
         <v>63</v>
       </c>
       <c r="H2" s="5"/>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="12" t="s">
         <v>2</v>
       </c>
     </row>
@@ -6898,13 +6910,13 @@
       <c r="J11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="13" t="s">
+      <c r="N11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="P11" s="13" t="s">
+      <c r="P11" s="12" t="s">
         <v>21</v>
       </c>
     </row>
@@ -7035,7 +7047,7 @@
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>53</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -7062,7 +7074,7 @@
       <c r="J19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L19" s="13" t="s">
+      <c r="L19" s="12" t="s">
         <v>34</v>
       </c>
       <c r="N19" s="5"/>
@@ -7101,7 +7113,9 @@
       <c r="L21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N21" s="4"/>
+      <c r="N21" s="12" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="F22" s="1" t="s">
@@ -7116,10 +7130,12 @@
       <c r="L22" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="N22" s="4"/>
+      <c r="N22" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="12" t="s">
         <v>92</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -7131,7 +7147,9 @@
       <c r="L23" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="N23" s="4"/>
+      <c r="N23" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="D24" s="1" t="s">
@@ -7143,7 +7161,9 @@
       <c r="L24" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="N24" s="4"/>
+      <c r="N24" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
@@ -7161,7 +7181,9 @@
       <c r="L25" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="N25" s="4"/>
+      <c r="N25" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
@@ -7179,6 +7201,9 @@
       <c r="L26" s="3" t="s">
         <v>136</v>
       </c>
+      <c r="N26" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
@@ -7190,6 +7215,9 @@
       <c r="L27" s="3" t="s">
         <v>137</v>
       </c>
+      <c r="N27" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
@@ -7274,7 +7302,7 @@
       <c r="H33" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="L33" s="13" t="s">
+      <c r="L33" s="12" t="s">
         <v>44</v>
       </c>
     </row>
@@ -7285,7 +7313,7 @@
       <c r="H34" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J34" s="13" t="s">
+      <c r="J34" s="12" t="s">
         <v>81</v>
       </c>
       <c r="L34" s="1" t="s">
@@ -7369,20 +7397,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="12"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="J5" s="12" t="s">
+      <c r="E5" s="13"/>
+      <c r="J5" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="K5" s="12"/>
+      <c r="K5" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="150" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
@@ -7434,6 +7462,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007C7BC51C6935E24091EF0B914732203F" ma:contentTypeVersion="10" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="0c86b061916a4edf5969eccf70c667b6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="71c32d65-301a-444d-ab8c-03b94330fe6c" xmlns:ns4="33cffe65-8a2d-4e1b-84ea-f2a734a98433" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5a93e4c052d79abae0fd6ae4db933211" ns3:_="" ns4:_="">
     <xsd:import namespace="71c32d65-301a-444d-ab8c-03b94330fe6c"/>
@@ -7636,22 +7679,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{161729E1-CF4C-47C3-80E6-567C9784CB01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56784C18-FCB8-4E15-8090-4487949A38C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B376350-3CA7-4FF1-919E-A559410F3184}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7668,21 +7713,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56784C18-FCB8-4E15-8090-4487949A38C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{161729E1-CF4C-47C3-80E6-567C9784CB01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>